<commit_message>
Updated AndroidNotes docx and BookTeraIssues xlsx
</commit_message>
<xml_diff>
--- a/Helpers/BookTera issues.xlsx
+++ b/Helpers/BookTera issues.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="76">
   <si>
     <t>Added</t>
   </si>
@@ -236,6 +236,12 @@
   </si>
   <si>
     <t>BookBlock.fill -&gt; ellenőrizni, h jók-e az 'if'-ek</t>
+  </si>
+  <si>
+    <t>Megoldottam inkább csalással</t>
+  </si>
+  <si>
+    <t>Search page: a textbox végén legyen nagyító is</t>
   </si>
 </sst>
 </file>
@@ -611,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S974"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1490,25 +1496,29 @@
       <c r="M42" s="12"/>
       <c r="N42" s="12"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B43" s="2" t="s">
+    <row r="43" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="4">
         <v>42044</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="D43" s="4">
+        <v>42056</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H43" s="12" t="s">
+      <c r="G43" s="4"/>
+      <c r="H43" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="I43" s="12"/>
-      <c r="J43" s="12"/>
-      <c r="K43" s="12"/>
-      <c r="L43" s="12"/>
-      <c r="M43" s="12"/>
-      <c r="N43" s="12"/>
+      <c r="J43" s="5" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
@@ -1530,27 +1540,33 @@
       <c r="M44" s="12"/>
       <c r="N44" s="12"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B45" s="2" t="s">
+    <row r="45" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="1">
-        <v>42044</v>
-      </c>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
+      <c r="C45" s="4">
+        <v>42056</v>
+      </c>
+      <c r="D45" s="4">
+        <v>42056</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G45" s="4"/>
+      <c r="H45" s="5" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C46" s="1">
-        <v>42044</v>
+        <v>42056</v>
       </c>
       <c r="H46" s="12"/>
       <c r="I46" s="12"/>
@@ -1565,7 +1581,7 @@
         <v>7</v>
       </c>
       <c r="C47" s="1">
-        <v>42044</v>
+        <v>42056</v>
       </c>
       <c r="H47" s="12"/>
       <c r="I47" s="12"/>
@@ -1580,7 +1596,7 @@
         <v>7</v>
       </c>
       <c r="C48" s="1">
-        <v>42044</v>
+        <v>42056</v>
       </c>
       <c r="H48" s="12"/>
       <c r="I48" s="12"/>
@@ -1595,7 +1611,7 @@
         <v>7</v>
       </c>
       <c r="C49" s="1">
-        <v>42044</v>
+        <v>42056</v>
       </c>
       <c r="H49" s="12"/>
       <c r="I49" s="12"/>
@@ -1610,7 +1626,7 @@
         <v>7</v>
       </c>
       <c r="C50" s="1">
-        <v>42044</v>
+        <v>42056</v>
       </c>
       <c r="H50" s="12"/>
       <c r="I50" s="12"/>
@@ -1625,7 +1641,7 @@
         <v>7</v>
       </c>
       <c r="C51" s="1">
-        <v>42044</v>
+        <v>42056</v>
       </c>
       <c r="H51" s="12"/>
       <c r="I51" s="12"/>
@@ -1640,7 +1656,7 @@
         <v>7</v>
       </c>
       <c r="C52" s="1">
-        <v>42044</v>
+        <v>42056</v>
       </c>
       <c r="H52" s="12"/>
       <c r="I52" s="12"/>
@@ -1655,7 +1671,7 @@
         <v>7</v>
       </c>
       <c r="C53" s="1">
-        <v>42044</v>
+        <v>42056</v>
       </c>
       <c r="H53" s="12"/>
       <c r="I53" s="12"/>
@@ -1670,7 +1686,7 @@
         <v>7</v>
       </c>
       <c r="C54" s="1">
-        <v>42044</v>
+        <v>42056</v>
       </c>
       <c r="H54" s="12"/>
       <c r="I54" s="12"/>
@@ -1685,7 +1701,7 @@
         <v>7</v>
       </c>
       <c r="C55" s="1">
-        <v>42044</v>
+        <v>42056</v>
       </c>
       <c r="H55" s="12"/>
       <c r="I55" s="12"/>
@@ -1700,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="C56" s="1">
-        <v>42044</v>
+        <v>42056</v>
       </c>
       <c r="H56" s="12"/>
       <c r="I56" s="12"/>
@@ -1715,7 +1731,7 @@
         <v>7</v>
       </c>
       <c r="C57" s="1">
-        <v>42044</v>
+        <v>42056</v>
       </c>
       <c r="H57" s="12"/>
       <c r="I57" s="12"/>

</xml_diff>

<commit_message>
Added Screenshots and Diagrams (into Helpers)
</commit_message>
<xml_diff>
--- a/Helpers/BookTera issues.xlsx
+++ b/Helpers/BookTera issues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="8520"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="8520" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BookTera" sheetId="6" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="158">
   <si>
     <t>Added</t>
   </si>
@@ -869,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S961"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2274,7 +2274,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="65" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
         <v>7</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
         <v>5</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="67" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
         <v>5</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="68" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
         <v>5</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="69" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
         <v>5</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="70" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
         <v>5</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="71" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
         <v>5</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="72" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
         <v>5</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="73" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
         <v>5</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="74" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
         <v>22</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="75" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
         <v>5</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="76" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
         <v>5</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="77" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="s">
         <v>5</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="78" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
         <v>5</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="79" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
         <v>5</v>
       </c>
@@ -2581,24 +2581,26 @@
         <v>149</v>
       </c>
     </row>
-    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B80" s="2" t="s">
+    <row r="80" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C80" s="1">
+      <c r="C80" s="4">
         <v>42107</v>
       </c>
-      <c r="F80" s="1" t="s">
+      <c r="D80" s="4">
+        <v>42125</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F80" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H80" s="12" t="s">
+      <c r="G80" s="4"/>
+      <c r="H80" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="J80" s="12"/>
-      <c r="K80" s="12"/>
-      <c r="L80" s="12"/>
-      <c r="M80" s="12"/>
-      <c r="N80" s="12"/>
     </row>
     <row r="81" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
@@ -29300,8 +29302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N891"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29365,25 +29367,26 @@
       <c r="M4" s="16"/>
       <c r="N4" s="16"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>42078</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="D5" s="4">
+        <v>42125</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="G5" s="4"/>
+      <c r="H5" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
     </row>
     <row r="6" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
@@ -29406,25 +29409,26 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+    <row r="7" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="4">
         <v>42078</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="D7" s="4">
+        <v>42125</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="G7" s="4"/>
+      <c r="H7" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">

</xml_diff>

<commit_message>
Updated Helpers (readme.md, SpeedTest)
</commit_message>
<xml_diff>
--- a/Helpers/BookTera issues.xlsx
+++ b/Helpers/BookTera issues.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="159">
   <si>
     <t>Added</t>
   </si>
@@ -491,6 +491,9 @@
   <si>
     <t>WebPlay: Az ASPXAUTH süti nem HTTPOnly</t>
   </si>
+  <si>
+    <t>Readme-be rendes leírás (akor az Install Guidelines-ből is copy-zható szöveg)</t>
+  </si>
 </sst>
 </file>
 
@@ -548,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -562,10 +565,6 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -29303,7 +29302,7 @@
   <dimension ref="B2:N891"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29344,28 +29343,26 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
+    <row r="4" spans="2:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="7">
         <v>42073</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15" t="s">
+      <c r="D4" s="7">
+        <v>42141</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="16" t="s">
+      <c r="G4" s="7"/>
+      <c r="H4" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
     </row>
     <row r="5" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -29430,48 +29427,61 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+    <row r="8" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <v>42078</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="D8" s="4">
+        <v>42141</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="G8" s="4"/>
+      <c r="H8" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+    </row>
+    <row r="9" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="4">
         <v>42078</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="D9" s="4">
+        <v>42141</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="G9" s="4"/>
+      <c r="H9" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H10" s="12"/>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1">
+        <v>42141</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>158</v>
+      </c>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
@@ -42582,6 +42592,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>